<commit_message>
add duplicate check and edit source on doubleclick
</commit_message>
<xml_diff>
--- a/src/output/output.xlsx
+++ b/src/output/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>dodid</t>
   </si>
@@ -67,12 +67,6 @@
     <t>johncena</t>
   </si>
   <si>
-    <t>nicholasfletcher</t>
-  </si>
-  <si>
-    <t>jcena</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -83,12 +77,6 @@
   </si>
   <si>
     <t>John Cena</t>
-  </si>
-  <si>
-    <t>Nicholas Fletcher</t>
-  </si>
-  <si>
-    <t>J Cena</t>
   </si>
 </sst>
 </file>
@@ -482,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -541,7 +529,7 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <f>CHOOSE(1,"","IND_OVERDUE")</f>
@@ -588,7 +576,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -607,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"","IND_ASSIGNED")</f>
         <v>0</v>
       </c>
       <c r="J3">
@@ -629,13 +617,13 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
-        <v>-1</v>
+        <v>4453245321</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -650,19 +638,19 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>CHOOSE(1,"","IND_ASSIGNED")</f>
+        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"2024-08-28","IND_OVERDUE")</f>
         <v>0</v>
       </c>
       <c r="L4">
@@ -670,34 +658,34 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"2000-01-01","IND_ONTIME")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
-        <v>-1</v>
+        <v>5555555555</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
       <c r="I5">
@@ -713,444 +701,21 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
         <v>0</v>
       </c>
       <c r="M5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6">
-        <v>-1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7">
-        <v>-1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8">
-        <v>-1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <f>CHOOSE(1,"2024-08-28","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>-1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10">
-        <v>-1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11">
-        <v>-1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12">
-        <v>-1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13">
-        <v>4453245321</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <f>CHOOSE(1,"2000-01-01","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14">
-        <v>5555555555</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M14">
         <f>CHOOSE(1,"2000-01-01","IND_OVERDUE")</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E14">
+  <conditionalFormatting sqref="A2:E5">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>AND(COLUMN(A2) &lt; 5, ROW(A2) &lt; 15)</formula>
+      <formula>AND(COLUMN(A2) &lt; 5, ROW(A2) &lt; 6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:M14">
+  <conditionalFormatting sqref="E2:M5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISNUMBER(SEARCH("IND_OVERDUE", _xlfn.FORMULATEXT(E2)))</formula>
     </cfRule>

</xml_diff>